<commit_message>
commit du fichier test
</commit_message>
<xml_diff>
--- a/front-end/tests/test.xlsx
+++ b/front-end/tests/test.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -879,27 +880,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1498,7 +1499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A60" sqref="A60:A62"/>
     </sheetView>
   </sheetViews>
@@ -1569,10 +1570,10 @@
       <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1584,56 +1585,56 @@
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="23"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="18"/>
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="18"/>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="23"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="18"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="18"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="23"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18"/>
       <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
@@ -1656,219 +1657,219 @@
       <c r="A14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="19"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="24" customHeight="1">
       <c r="A15" s="18"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1">
       <c r="A16" s="18"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" ht="24" customHeight="1">
       <c r="A17" s="18"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1">
       <c r="A19" s="18"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="60" customHeight="1">
       <c r="A20" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="21"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="20"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" ht="45">
       <c r="A25" s="18"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="20"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="1:5" ht="30">
       <c r="A27" s="18"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="20"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="18"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="20"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" ht="45">
       <c r="A29" s="18"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="21"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:5" ht="45">
       <c r="A30" s="18"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="21"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="20"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="18"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="21"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="18"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="21"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5" ht="30">
       <c r="A33" s="18"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="21"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="20"/>
+      <c r="E33" s="26"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="21"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="20"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:5" ht="30">
       <c r="A35" s="18"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="21"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="20"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="21"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="20"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="20"/>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="18" t="s">
@@ -2007,30 +2008,35 @@
       <c r="A60" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D60" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="18"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="24"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="20"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="18"/>
-      <c r="B62" s="22"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="24"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="E20:E37"/>
+    <mergeCell ref="C20:C37"/>
+    <mergeCell ref="B20:B37"/>
+    <mergeCell ref="A20:A37"/>
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="D60:D62"/>
@@ -2044,11 +2050,6 @@
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A43:A45"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="E20:E37"/>
-    <mergeCell ref="C20:C37"/>
-    <mergeCell ref="B20:B37"/>
-    <mergeCell ref="A20:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>